<commit_message>
[ADD] Brake version 2
</commit_message>
<xml_diff>
--- a/parameters/RS12.xlsx
+++ b/parameters/RS12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Desktop\TIA\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08131F94-401C-4CB1-90F8-F85178F7FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F18BB1-4503-47FC-A8D2-BD64354330BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="2265" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Front</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>Pedal ratio</t>
+  </si>
+  <si>
+    <t>Master cylider cross section area</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A11" sqref="A11:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,6 +667,62 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E10" s="6"/>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[ADD] New version of BrakeAbaqus
</commit_message>
<xml_diff>
--- a/parameters/RS12.xlsx
+++ b/parameters/RS12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Desktop\TIA\parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\TIA\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12169668-884E-4752-A4FC-9A967050F9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3370AF13-5805-4C02-99D6-FF49D0739A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="2130" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8670" yWindow="1905" windowWidth="16125" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -239,6 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
@@ -523,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +535,7 @@
     <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -546,7 +547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -561,12 +562,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>2.67</v>
+        <v>3.32</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -576,15 +577,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>1.98</v>
+        <v>3.87</v>
       </c>
       <c r="C4" s="3">
-        <v>1.98</v>
+        <v>3.87</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -593,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -610,7 +611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -627,7 +628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -644,7 +645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -661,21 +662,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -683,7 +685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -691,7 +693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -699,7 +701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -707,7 +709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>